<commit_message>
Consolidated user made libraries and added components for V3.
</commit_message>
<xml_diff>
--- a/Parts/Componet List.xlsx
+++ b/Parts/Componet List.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77b7aaadc6b9f2e9/Documents/GitHub/DBF/PCB-Shield-Design/Parts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\GitHub\DBF\PCB-Shield-Design\Parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="8_{67CA6F16-8642-40DE-87EA-04BBB26B3169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CD49381-35F9-45B4-8AF7-01C1A89F6252}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11536BF7-30BB-40E7-844D-7C4B6D681F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A63A2686-3B4E-457C-A8F5-34C06D046AA0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A63A2686-3B4E-457C-A8F5-34C06D046AA0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PCB_Shield_v2" sheetId="1" r:id="rId1"/>
+    <sheet name="PCB_Shield_v3" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
   <si>
     <t>Componet Name</t>
   </si>
@@ -193,6 +194,63 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-3EKF66R5V/196443?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbXABYAGANjJAF18AHAFyhAGVmAnASwDsA5iAC%2B%2BAMzwQSSGix5CJcGDEQGIFm069BI-GCqTpsnPiKRSYgJwwyBtRsgdu-IaJAwKADgCshlBhMFcxAqKgA6bwACAHkACwBbTHomVkcAVT4eZmjkAFlsVEwAVy5sXRAAWghoKX85U0UwCno3Crga6W4i%2BTNSXzphN3bSUsweTGYCLhagA</t>
+  </si>
+  <si>
+    <t>Part #</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Spec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qty </t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>In Altium</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
+  </si>
+  <si>
+    <t>TSR 1-2450</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/traco-power/TSR-1-2450/9383780</t>
+  </si>
+  <si>
+    <t>5V 1A Output</t>
+  </si>
+  <si>
+    <t>Buck Converter</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Need to Order (Y/N)</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>https://www.tracopower.com/sites/default/files/products/datasheets/tsr1_datasheet.pdf</t>
+  </si>
+  <si>
+    <t>XT30 right angle connector</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Amass-XT30PW-Upgrade-Connectors-Battery/dp/B099F2PXYN/ref=sr_1_1?crid=1HAEZSSILG0HP&amp;keywords=XT30+right+angle+connector&amp;qid=1643672653&amp;sprefix=xt30+right+angle+connector%2Caps%2C116&amp;sr=8-1</t>
+  </si>
+  <si>
+    <t>XT30</t>
+  </si>
+  <si>
+    <t>Avionics Battery Connector</t>
   </si>
 </sst>
 </file>
@@ -589,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C94F46-05EA-4C66-9DE9-87932AFAEECC}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -936,4 +994,115 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId14"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC095FF6-77C3-4985-9DFF-126D085E00A0}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>